<commit_message>
var data types and constants
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bagew\Desktop\WebDev\Kotlin_android\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{656A4467-0EB8-4663-B3ED-98B927284E01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A7D4061-7FE6-438E-889C-2D7EA02BFF02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9852" yWindow="0" windowWidth="13188" windowHeight="12240" xr2:uid="{17B742CA-5D3D-4D18-9A28-142DB084ECCD}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t xml:space="preserve">Kotlin_Android RoadMap </t>
   </si>
@@ -54,7 +54,10 @@
     <t>StartDate</t>
   </si>
   <si>
-    <t>BasicStructure of Kotlin</t>
+    <t>BasicStructure of Kotlin in comparision to java</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Variable, DataTypes and Constants </t>
   </si>
 </sst>
 </file>
@@ -113,7 +116,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -123,6 +126,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -440,12 +452,13 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="33.44140625" customWidth="1"/>
+    <col min="3" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -473,21 +486,31 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="3">
+    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="5">
         <v>1</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
+      <c r="C5" s="7">
+        <v>45869</v>
+      </c>
+      <c r="D5" s="7">
+        <v>45869</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
+      <c r="A6" s="5">
+        <v>2</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="7">
+        <v>45869</v>
+      </c>
+      <c r="D6" s="5"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>

</xml_diff>